<commit_message>
updated sample excel file as Id was not fine
</commit_message>
<xml_diff>
--- a/jcp-v2/04-rsconnectProfiles/SKUs_0403.xlsx
+++ b/jcp-v2/04-rsconnectProfiles/SKUs_0403.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\#SrcCode\GitHub-RS\dataplatform-sampledata\jcp-v2\04-rsconnectProfiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RS\dataplatform-sampledata\jcp-v2\04-rsconnectProfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Display Name</t>
   </si>
@@ -66,12 +66,18 @@
   </si>
   <si>
     <t>Id</t>
+  </si>
+  <si>
+    <t>JImport1</t>
+  </si>
+  <si>
+    <t>Jimport2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -196,6 +202,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -231,6 +254,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -387,17 +427,17 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="4" width="31.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="4" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -420,9 +460,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>8989898982</v>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -443,9 +483,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>8989898981</v>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>

</xml_diff>